<commit_message>
Uprava aplikace, nove statistiky
</commit_message>
<xml_diff>
--- a/prace/charts.xlsx
+++ b/prace/charts.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\agent\Documents\Projekty\dopravni-znacky\prace\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44437C67-8C85-477F-B0E6-4F83BAABC161}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90EE79B2-A715-4BCD-AF66-12D59C57478D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13695" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13695" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Podíl zdrojů dat" sheetId="1" r:id="rId1"/>
+    <sheet name="Výkon na zařízeních" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="39">
   <si>
     <t>Zdroj</t>
   </si>
@@ -73,13 +74,102 @@
   <si>
     <t>Podíl (r:g)</t>
   </si>
+  <si>
+    <t>Zařízení</t>
+  </si>
+  <si>
+    <t>SSD Mobilenet 320x320</t>
+  </si>
+  <si>
+    <t>SSD Mobilenet 640x480</t>
+  </si>
+  <si>
+    <t>SSD Mobilenet 320x320 (quantized)</t>
+  </si>
+  <si>
+    <t>SSD Mobilenet 640x480 (quantized)</t>
+  </si>
+  <si>
+    <t>SSD Mobilenet FPNlite 640x480</t>
+  </si>
+  <si>
+    <t>SSD EfficentDet 512x512</t>
+  </si>
+  <si>
+    <t>Samsung galaxy M11</t>
+  </si>
+  <si>
+    <t>Rok výroby</t>
+  </si>
+  <si>
+    <t>~12FPS</t>
+  </si>
+  <si>
+    <t>~8FPS</t>
+  </si>
+  <si>
+    <t>~3FPS</t>
+  </si>
+  <si>
+    <t>~2FPS</t>
+  </si>
+  <si>
+    <t>&lt;0.5FPS</t>
+  </si>
+  <si>
+    <t>~10FPS</t>
+  </si>
+  <si>
+    <t>~4FPS</t>
+  </si>
+  <si>
+    <t>~30-40FPS</t>
+  </si>
+  <si>
+    <t>~18FPS</t>
+  </si>
+  <si>
+    <t>~1.5FPS</t>
+  </si>
+  <si>
+    <t>Xiaomi Redmi Note 11 S</t>
+  </si>
+  <si>
+    <t>~52FPS</t>
+  </si>
+  <si>
+    <t>Intel i5-11320H</t>
+  </si>
+  <si>
+    <t>~14FPS</t>
+  </si>
+  <si>
+    <t>~7FPS</t>
+  </si>
+  <si>
+    <t>Model</t>
+  </si>
+  <si>
+    <t>Normální</t>
+  </si>
+  <si>
+    <t>Quantizovaný</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -116,16 +206,41 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normální" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -805,6 +920,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-1216-4F1D-A0BC-14549B155C7E}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
@@ -820,6 +940,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-1216-4F1D-A0BC-14549B155C7E}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
@@ -835,6 +960,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-1216-4F1D-A0BC-14549B155C7E}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="3"/>
@@ -850,6 +980,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-1216-4F1D-A0BC-14549B155C7E}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:cat>
             <c:strRef>
@@ -957,6 +1092,1189 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="cs-CZ"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="cs-CZ"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="cs-CZ"/>
+              <a:t>Rychlost na různých</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="cs-CZ" baseline="0"/>
+              <a:t> zařízeních(FPS)</a:t>
+            </a:r>
+            <a:endParaRPr lang="cs-CZ"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="cs-CZ"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Výkon na zařízeních'!$B$17</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Samsung galaxy M11</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Výkon na zařízeních'!$C$16:$H$16</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>SSD Mobilenet 320x320</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>SSD Mobilenet 640x480</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>SSD Mobilenet 320x320 (quantized)</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>SSD Mobilenet 640x480 (quantized)</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>SSD Mobilenet FPNlite 640x480</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>SSD EfficentDet 512x512</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Výkon na zařízeních'!$C$17:$H$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-FCD1-4550-A1CE-2584523A14EA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Výkon na zařízeních'!$B$18</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Xiaomi Redmi Note 11 S</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Výkon na zařízeních'!$C$16:$H$16</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>SSD Mobilenet 320x320</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>SSD Mobilenet 640x480</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>SSD Mobilenet 320x320 (quantized)</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>SSD Mobilenet 640x480 (quantized)</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>SSD Mobilenet FPNlite 640x480</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>SSD EfficentDet 512x512</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Výkon na zařízeních'!$C$18:$H$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-FCD1-4550-A1CE-2584523A14EA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Výkon na zařízeních'!$B$23</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Intel i5-11320H</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Výkon na zařízeních'!$C$16:$H$16</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>SSD Mobilenet 320x320</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>SSD Mobilenet 640x480</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>SSD Mobilenet 320x320 (quantized)</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>SSD Mobilenet 640x480 (quantized)</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>SSD Mobilenet FPNlite 640x480</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>SSD EfficentDet 512x512</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Výkon na zařízeních'!$C$23:$H$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-FCD1-4550-A1CE-2584523A14EA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Výkon na zařízeních'!#REF!</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>#REF!</c:v>
+                </c:pt>
+              </c:strCache>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:lumMod val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Výkon na zařízeních'!$C$16:$H$16</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>SSD Mobilenet 320x320</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>SSD Mobilenet 640x480</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>SSD Mobilenet 320x320 (quantized)</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>SSD Mobilenet 640x480 (quantized)</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>SSD Mobilenet FPNlite 640x480</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>SSD EfficentDet 512x512</c:v>
+                </c:pt>
+              </c:strCache>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Výkon na zařízeních'!#REF!</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
+            </c:numRef>
+          </c:val>
+          <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-FCD1-4550-A1CE-2584523A14EA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="665344848"/>
+        <c:axId val="665342928"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredBarSeries>
+              <c15:ser>
+                <c:idx val="3"/>
+                <c:order val="3"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'Výkon na zařízeních'!$B$20</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:solidFill>
+                    <a:schemeClr val="accent4"/>
+                  </a:solidFill>
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:invertIfNegative val="0"/>
+                <c:cat>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'Výkon na zařízeních'!$C$16:$H$16</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="6"/>
+                      <c:pt idx="0">
+                        <c:v>SSD Mobilenet 320x320</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>SSD Mobilenet 640x480</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>SSD Mobilenet 320x320 (quantized)</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>SSD Mobilenet 640x480 (quantized)</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>SSD Mobilenet FPNlite 640x480</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>SSD EfficentDet 512x512</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'Výkon na zařízeních'!$C$20:$H$20</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="6"/>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000003-FCD1-4550-A1CE-2584523A14EA}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredBarSeries>
+            <c15:filteredBarSeries>
+              <c15:ser>
+                <c:idx val="4"/>
+                <c:order val="4"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'Výkon na zařízeních'!$B$21</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:solidFill>
+                    <a:schemeClr val="accent5"/>
+                  </a:solidFill>
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:invertIfNegative val="0"/>
+                <c:cat>
+                  <c:strRef>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'Výkon na zařízeních'!$C$16:$H$16</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="6"/>
+                      <c:pt idx="0">
+                        <c:v>SSD Mobilenet 320x320</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>SSD Mobilenet 640x480</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>SSD Mobilenet 320x320 (quantized)</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>SSD Mobilenet 640x480 (quantized)</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>SSD Mobilenet FPNlite 640x480</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>SSD EfficentDet 512x512</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'Výkon na zařízeních'!$C$21:$H$21</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="6"/>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000004-FCD1-4550-A1CE-2584523A14EA}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredBarSeries>
+            <c15:filteredBarSeries>
+              <c15:ser>
+                <c:idx val="5"/>
+                <c:order val="5"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'Výkon na zařízeních'!$B$22</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:solidFill>
+                    <a:schemeClr val="accent6"/>
+                  </a:solidFill>
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:invertIfNegative val="0"/>
+                <c:cat>
+                  <c:strRef>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'Výkon na zařízeních'!$C$16:$H$16</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="6"/>
+                      <c:pt idx="0">
+                        <c:v>SSD Mobilenet 320x320</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>SSD Mobilenet 640x480</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>SSD Mobilenet 320x320 (quantized)</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>SSD Mobilenet 640x480 (quantized)</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>SSD Mobilenet FPNlite 640x480</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>SSD EfficentDet 512x512</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'Výkon na zařízeních'!$C$22:$H$22</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="6"/>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000005-FCD1-4550-A1CE-2584523A14EA}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredBarSeries>
+          </c:ext>
+        </c:extLst>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="665344848"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="cs-CZ"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="665342928"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="665342928"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="cs-CZ"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="665344848"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="cs-CZ"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="cs-CZ"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="cs-CZ"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Výkon na zařízeních'!$M$16</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Normální</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Výkon na zařízeních'!$L$17:$L$18</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>SSD Mobilenet 640x480</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>SSD Mobilenet 320x320</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Výkon na zařízeních'!$M$17:$M$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-B729-4591-80DC-3D359BFDFCA0}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Výkon na zařízeních'!$N$16</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Quantizovaný</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Výkon na zařízeních'!$L$17:$L$18</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>SSD Mobilenet 640x480</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>SSD Mobilenet 320x320</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Výkon na zařízeních'!$N$17:$N$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>23.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-B729-4591-80DC-3D359BFDFCA0}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="182"/>
+        <c:axId val="266679007"/>
+        <c:axId val="266678047"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="266679007"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="cs-CZ"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="266678047"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="266678047"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="cs-CZ"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="266679007"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="cs-CZ"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
@@ -1112,6 +2430,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="251">
   <cs:axisTitle>
@@ -2327,6 +3725,1014 @@
       <cs:styleClr val="auto"/>
     </cs:lnRef>
     <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
@@ -2782,6 +5188,100 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>625071</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>20443</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>44079</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>79607</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Graf 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4222BDC7-C760-D002-147A-1D423C4CBF74}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>169420</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>61051</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>439554</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>110707</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Graf 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{711F6B1E-82AF-3BBC-38DA-0D971FE8CF5E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DCFC5C40-A6D9-4B94-B02F-755279A155DA}" name="Tabulka1" displayName="Tabulka1" ref="B2:I11" totalsRowShown="0" headerRowDxfId="1" headerRowBorderDxfId="0">
+  <autoFilter ref="B2:I11" xr:uid="{DCFC5C40-A6D9-4B94-B02F-755279A155DA}"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{98BA6C80-F794-4AED-8F9B-6201B6A911AE}" name="Zařízení"/>
+    <tableColumn id="2" xr3:uid="{DBBDC7DD-DB2E-460D-A5CC-E2D9329AC318}" name="Rok výroby"/>
+    <tableColumn id="3" xr3:uid="{074EEB62-1DF9-4B23-95BA-373402CA1896}" name="SSD Mobilenet 320x320"/>
+    <tableColumn id="4" xr3:uid="{3108B529-906F-465D-BA58-24003F966203}" name="SSD Mobilenet 640x480"/>
+    <tableColumn id="5" xr3:uid="{BE00D442-9568-41D6-AD39-F45B0028A338}" name="SSD Mobilenet 320x320 (quantized)"/>
+    <tableColumn id="6" xr3:uid="{0D84F257-7DBF-4E4D-B36F-D1C457792501}" name="SSD Mobilenet 640x480 (quantized)"/>
+    <tableColumn id="7" xr3:uid="{5470D79E-E44C-4F54-B931-719CB8C2C7DE}" name="SSD Mobilenet FPNlite 640x480"/>
+    <tableColumn id="8" xr3:uid="{DD3DE702-3751-4FE5-9F6F-94291BD79611}" name="SSD EfficentDet 512x512"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -3047,8 +5547,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:S8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3085,52 +5585,52 @@
       </c>
     </row>
     <row r="3" spans="2:19" x14ac:dyDescent="0.45">
-      <c r="B3" s="1" t="s">
+      <c r="B3" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3">
         <f>S6</f>
         <v>355</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="J3" t="s">
         <v>5</v>
       </c>
-      <c r="K3" s="1">
+      <c r="K3">
         <f>L3*2</f>
         <v>280</v>
       </c>
-      <c r="L3" s="1">
+      <c r="L3">
         <v>140</v>
       </c>
-      <c r="R3" s="1" t="s">
+      <c r="R3" t="s">
         <v>5</v>
       </c>
-      <c r="S3" s="1">
+      <c r="S3">
         <v>56</v>
       </c>
     </row>
     <row r="4" spans="2:19" x14ac:dyDescent="0.45">
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="1">
         <f>K8</f>
         <v>2288</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="J4" t="s">
         <v>2</v>
       </c>
-      <c r="K4" s="1">
+      <c r="K4">
         <f>L4*2</f>
         <v>324</v>
       </c>
-      <c r="L4" s="1">
+      <c r="L4">
         <v>162</v>
       </c>
-      <c r="R4" s="1" t="s">
+      <c r="R4" t="s">
         <v>2</v>
       </c>
-      <c r="S4" s="1">
+      <c r="S4">
         <v>232</v>
       </c>
     </row>
@@ -3142,19 +5642,19 @@
         <f>SUM(C3:C4)</f>
         <v>2643</v>
       </c>
-      <c r="J5" s="1" t="s">
+      <c r="J5" t="s">
         <v>7</v>
       </c>
-      <c r="K5" s="1">
+      <c r="K5">
         <v>500</v>
       </c>
-      <c r="L5" s="1">
+      <c r="L5">
         <v>500</v>
       </c>
-      <c r="R5" s="2" t="s">
+      <c r="R5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="S5" s="2">
+      <c r="S5" s="1">
         <v>67</v>
       </c>
     </row>
@@ -3166,17 +5666,17 @@
         <f>_xlfn.CONCAT(1, ":", ROUND(C4/C3,1))</f>
         <v>1:6.4</v>
       </c>
-      <c r="J6" s="2" t="s">
+      <c r="J6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="K6" s="2">
+      <c r="K6" s="1">
         <f>L6*2</f>
         <v>40</v>
       </c>
-      <c r="L6" s="2">
+      <c r="L6" s="1">
         <v>20</v>
       </c>
-      <c r="R6" s="3" t="s">
+      <c r="R6" t="s">
         <v>10</v>
       </c>
       <c r="S6">
@@ -3207,4 +5707,258 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8505E0B5-EEF7-4EE8-9327-162CF4AE596A}">
+  <dimension ref="B2:N23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="F9" zoomScale="68" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Q38" sqref="Q38"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="2" max="2" width="29.796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.1328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="33.06640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="29.53125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.796875" customWidth="1"/>
+    <col min="12" max="12" width="19.9296875" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="15.59765625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:14" x14ac:dyDescent="0.45">
+      <c r="B2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="2:14" x14ac:dyDescent="0.45">
+      <c r="B3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3">
+        <v>2020</v>
+      </c>
+      <c r="D3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H3" t="s">
+        <v>24</v>
+      </c>
+      <c r="I3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="2:14" x14ac:dyDescent="0.45">
+      <c r="B4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4">
+        <v>2022</v>
+      </c>
+      <c r="D4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F4" t="s">
+        <v>28</v>
+      </c>
+      <c r="G4" t="s">
+        <v>29</v>
+      </c>
+      <c r="H4" t="s">
+        <v>27</v>
+      </c>
+      <c r="I4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="2:14" x14ac:dyDescent="0.45">
+      <c r="B5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5">
+        <v>2021</v>
+      </c>
+      <c r="D5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G5" t="s">
+        <v>27</v>
+      </c>
+      <c r="H5" t="s">
+        <v>34</v>
+      </c>
+      <c r="I5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="2:14" x14ac:dyDescent="0.45">
+      <c r="C16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D16" t="s">
+        <v>14</v>
+      </c>
+      <c r="E16" t="s">
+        <v>15</v>
+      </c>
+      <c r="F16" t="s">
+        <v>16</v>
+      </c>
+      <c r="G16" t="s">
+        <v>17</v>
+      </c>
+      <c r="H16" t="s">
+        <v>18</v>
+      </c>
+      <c r="L16" t="s">
+        <v>36</v>
+      </c>
+      <c r="M16" t="s">
+        <v>37</v>
+      </c>
+      <c r="N16" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="17" spans="2:14" x14ac:dyDescent="0.45">
+      <c r="B17" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17">
+        <v>8</v>
+      </c>
+      <c r="D17">
+        <v>3</v>
+      </c>
+      <c r="E17">
+        <v>12</v>
+      </c>
+      <c r="F17">
+        <v>8</v>
+      </c>
+      <c r="G17">
+        <v>2</v>
+      </c>
+      <c r="H17">
+        <v>0.5</v>
+      </c>
+      <c r="L17" t="s">
+        <v>14</v>
+      </c>
+      <c r="M17">
+        <f>AVERAGE(D17:D22)</f>
+        <v>3.5</v>
+      </c>
+      <c r="N17">
+        <f>AVERAGE(F17:F22)</f>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="2:14" x14ac:dyDescent="0.45">
+      <c r="B18" t="s">
+        <v>31</v>
+      </c>
+      <c r="C18">
+        <v>10</v>
+      </c>
+      <c r="D18">
+        <v>4</v>
+      </c>
+      <c r="E18">
+        <v>35</v>
+      </c>
+      <c r="F18">
+        <v>18</v>
+      </c>
+      <c r="G18">
+        <v>4</v>
+      </c>
+      <c r="H18">
+        <v>1.5</v>
+      </c>
+      <c r="L18" t="s">
+        <v>13</v>
+      </c>
+      <c r="M18">
+        <f>AVERAGE(C17:C22)</f>
+        <v>9</v>
+      </c>
+      <c r="N18">
+        <f>AVERAGE(E17:E22)</f>
+        <v>23.5</v>
+      </c>
+    </row>
+    <row r="23" spans="2:14" x14ac:dyDescent="0.45">
+      <c r="B23" t="s">
+        <v>33</v>
+      </c>
+      <c r="C23">
+        <v>52</v>
+      </c>
+      <c r="D23">
+        <v>18</v>
+      </c>
+      <c r="E23">
+        <v>3</v>
+      </c>
+      <c r="F23">
+        <v>4</v>
+      </c>
+      <c r="G23">
+        <v>14</v>
+      </c>
+      <c r="H23">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>